<commit_message>
Update customer report to v22
</commit_message>
<xml_diff>
--- a/reports/customers_list/template.xlsx
+++ b/reports/customers_list/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11220"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10224"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marc1/Documents/Connect/connect-cli/cnctcli/reports/connect-reports/reports/customers_list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC8D12E-66AE-9141-9077-86525BD00B3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CA801B-DE45-EC49-A49A-E620F9D54293}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35840" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$V$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$S$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Provider Name</t>
   </si>
@@ -80,15 +80,6 @@
   </si>
   <si>
     <t>Contact Phone number</t>
-  </si>
-  <si>
-    <t>Marketplace ID</t>
-  </si>
-  <si>
-    <t>Marketplace Name</t>
-  </si>
-  <si>
-    <t>Environment</t>
   </si>
   <si>
     <t>Extended Information</t>
@@ -438,34 +429,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="3" width="18" customWidth="1"/>
-    <col min="4" max="5" width="15.5" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="46.5" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="46.5" customWidth="1"/>
-    <col min="11" max="11" width="50.83203125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="15" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="14" width="46.1640625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="15" max="16" width="31" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="17" max="17" width="19.5" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="18" max="18" width="20" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="21" width="31.1640625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="22" max="22" width="25.6640625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="20.83203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="4" width="15.5" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="20" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="46.5" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="50.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="11" width="46.1640625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="13" width="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="19.5" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="20" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="18" width="31.1640625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="25.6640625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="20" width="20.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -473,71 +462,63 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V1" xr:uid="{444A851A-3A6C-984B-A410-97137E4DF2E6}"/>
+  <autoFilter ref="A1:S1" xr:uid="{444A851A-3A6C-984B-A410-97137E4DF2E6}"/>
+  <dataConsolidate/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>